<commit_message>
removed extra officers page file that did not work
</commit_message>
<xml_diff>
--- a/public/main_page/events_data.xlsx
+++ b/public/main_page/events_data.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\15413\Desktop\Alex\Projects\shpe_website\my_shpe_website\public\main_page\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\15413\Desktop\psu_shpe_website-main\psu_shpe_website-main\public\main_page\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6AA579E9-C0E2-4991-8FF2-05D3ACEB5287}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A09FFB88-20FF-4241-8A5A-4958CA28DA2B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="63705" yWindow="7365" windowWidth="28800" windowHeight="15225" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2280" yWindow="4150" windowWidth="28800" windowHeight="15370" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -109,7 +109,7 @@
     <t>Upcoming Events!</t>
   </si>
   <si>
-    <t>https://i.ibb.co/Zhq4zwz/grad-info-session-flyer.png</t>
+    <t>https://i.ibb.co/kKjmFRH/grad-info-session-flyer.png</t>
   </si>
 </sst>
 </file>
@@ -395,7 +395,7 @@
   <dimension ref="A1:E8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J18" sqref="J18"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6328125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>

</xml_diff>